<commit_message>
EDA Eliminação do Item Code 21016
</commit_message>
<xml_diff>
--- a/output/food_security_industry_features_analysis.xlsx
+++ b/output/food_security_industry_features_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dgarzao\git_repositories\202404_trabalho_ux\01_eda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dgarzao\git_repositories\202404_trabalho_ux\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCD3B4A-481D-4FED-959C-F493843408C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BA882B-B7B7-4A4D-B701-48D59491A852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="-11640" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="142">
   <si>
     <t>Item Code</t>
   </si>
@@ -446,6 +446,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>&lt;&lt;&lt; Brasil não tem</t>
   </si>
 </sst>
 </file>
@@ -843,11 +846,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1131,7 +1134,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
@@ -1148,7 +1151,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1165,7 +1168,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
@@ -1199,7 +1202,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
@@ -1284,7 +1287,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>52</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>54</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>56</v>
       </c>
@@ -1352,7 +1355,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>58</v>
       </c>
@@ -1369,7 +1372,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
@@ -1383,10 +1386,13 @@
         <v>1586</v>
       </c>
       <c r="E31" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="F31" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
EDA Food security industry final
</commit_message>
<xml_diff>
--- a/output/food_security_industry_features_analysis.xlsx
+++ b/output/food_security_industry_features_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\dgarzao\git_repositories\202404_trabalho_ux\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78BA882B-B7B7-4A4D-B701-48D59491A852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D41A9F6-6177-48E1-9A7E-B243625922D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="141">
   <si>
     <t>Item Code</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Number of people undernourished (million) (annual value)</t>
-  </si>
-  <si>
-    <t>210011</t>
   </si>
   <si>
     <t>Number of people undernourished (million) (3-year average)</t>
@@ -845,12 +842,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -893,15 +889,15 @@
         <v>1035</v>
       </c>
       <c r="E2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>210011</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="C3">
         <v>5227</v>
@@ -910,15 +906,15 @@
         <v>5227</v>
       </c>
       <c r="E3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C4">
         <v>1035</v>
@@ -927,15 +923,15 @@
         <v>1035</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="C5">
         <v>5229</v>
@@ -949,96 +945,96 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6">
+        <v>1215</v>
+      </c>
+      <c r="D6">
+        <v>1215</v>
+      </c>
+      <c r="E6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
-        <v>1215</v>
-      </c>
-      <c r="D6">
-        <v>1215</v>
-      </c>
-      <c r="E6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7">
+        <v>1215</v>
+      </c>
+      <c r="D7">
+        <v>1215</v>
+      </c>
+      <c r="E7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
-        <v>1215</v>
-      </c>
-      <c r="D7">
-        <v>1215</v>
-      </c>
-      <c r="E7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8">
+        <v>1215</v>
+      </c>
+      <c r="D8">
+        <v>1215</v>
+      </c>
+      <c r="E8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
-        <v>1215</v>
-      </c>
-      <c r="D8">
-        <v>1215</v>
-      </c>
-      <c r="E8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9">
+        <v>5229</v>
+      </c>
+      <c r="D9">
+        <v>5229</v>
+      </c>
+      <c r="E9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9">
-        <v>5229</v>
-      </c>
-      <c r="D9">
-        <v>5229</v>
-      </c>
-      <c r="E9" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10">
+        <v>5229</v>
+      </c>
+      <c r="D10">
+        <v>5229</v>
+      </c>
+      <c r="E10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10">
-        <v>5229</v>
-      </c>
-      <c r="D10">
-        <v>5229</v>
-      </c>
-      <c r="E10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="C11">
         <v>5229</v>
       </c>
@@ -1046,101 +1042,101 @@
         <v>5229</v>
       </c>
       <c r="E11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12">
+        <v>1215</v>
+      </c>
+      <c r="D12">
+        <v>1215</v>
+      </c>
+      <c r="E12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C12">
-        <v>1215</v>
-      </c>
-      <c r="D12">
-        <v>1215</v>
-      </c>
-      <c r="E12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13">
+        <v>1215</v>
+      </c>
+      <c r="D13">
+        <v>1215</v>
+      </c>
+      <c r="E13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C13">
-        <v>1215</v>
-      </c>
-      <c r="D13">
-        <v>1215</v>
-      </c>
-      <c r="E13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14">
+        <v>1215</v>
+      </c>
+      <c r="D14">
+        <v>1215</v>
+      </c>
+      <c r="E14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C14">
-        <v>1215</v>
-      </c>
-      <c r="D14">
-        <v>1215</v>
-      </c>
-      <c r="E14" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="B15" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15">
+        <v>5229</v>
+      </c>
+      <c r="D15">
+        <v>5229</v>
+      </c>
+      <c r="E15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C15">
-        <v>5229</v>
-      </c>
-      <c r="D15">
-        <v>5229</v>
-      </c>
-      <c r="E15" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="B16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16">
+        <v>5229</v>
+      </c>
+      <c r="D16">
+        <v>5229</v>
+      </c>
+      <c r="E16" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C16">
-        <v>5229</v>
-      </c>
-      <c r="D16">
-        <v>5229</v>
-      </c>
-      <c r="E16" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="C17">
         <v>5229</v>
       </c>
@@ -1148,50 +1144,50 @@
         <v>5229</v>
       </c>
       <c r="E17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18">
+        <v>1215</v>
+      </c>
+      <c r="D18">
+        <v>1215</v>
+      </c>
+      <c r="E18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C18">
-        <v>1215</v>
-      </c>
-      <c r="D18">
-        <v>1215</v>
-      </c>
-      <c r="E18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19">
+        <v>1215</v>
+      </c>
+      <c r="D19">
+        <v>1215</v>
+      </c>
+      <c r="E19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C19">
-        <v>1215</v>
-      </c>
-      <c r="D19">
-        <v>1215</v>
-      </c>
-      <c r="E19" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="B20" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="C20">
         <v>1215</v>
       </c>
@@ -1199,16 +1195,16 @@
         <v>1215</v>
       </c>
       <c r="E20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="C21">
         <v>1215</v>
       </c>
@@ -1216,16 +1212,16 @@
         <v>1215</v>
       </c>
       <c r="E21" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="C22">
         <v>1215</v>
       </c>
@@ -1233,67 +1229,67 @@
         <v>1215</v>
       </c>
       <c r="E22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23">
+        <v>1215</v>
+      </c>
+      <c r="D23">
+        <v>1215</v>
+      </c>
+      <c r="E23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C23">
-        <v>1215</v>
-      </c>
-      <c r="D23">
-        <v>1215</v>
-      </c>
-      <c r="E23" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24">
+        <v>5229</v>
+      </c>
+      <c r="D24">
+        <v>5229</v>
+      </c>
+      <c r="E24" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C24">
-        <v>5229</v>
-      </c>
-      <c r="D24">
-        <v>5229</v>
-      </c>
-      <c r="E24" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25">
+        <v>5229</v>
+      </c>
+      <c r="D25">
+        <v>5229</v>
+      </c>
+      <c r="E25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C25">
-        <v>5229</v>
-      </c>
-      <c r="D25">
-        <v>5229</v>
-      </c>
-      <c r="E25" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="C26">
         <v>5229</v>
       </c>
@@ -1301,15 +1297,15 @@
         <v>5229</v>
       </c>
       <c r="E26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>52</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>53</v>
       </c>
       <c r="C27">
         <v>4603</v>
@@ -1318,15 +1314,15 @@
         <v>4603</v>
       </c>
       <c r="E27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="C28">
         <v>4196</v>
@@ -1335,15 +1331,15 @@
         <v>4196</v>
       </c>
       <c r="E28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>56</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>57</v>
       </c>
       <c r="C29">
         <v>4229</v>
@@ -1352,15 +1348,15 @@
         <v>4229</v>
       </c>
       <c r="E29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="C30">
         <v>4229</v>
@@ -1369,15 +1365,15 @@
         <v>4229</v>
       </c>
       <c r="E30" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="C31">
         <v>1586</v>
@@ -1386,18 +1382,18 @@
         <v>1586</v>
       </c>
       <c r="E31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F31" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="C32">
         <v>4370</v>
@@ -1406,15 +1402,15 @@
         <v>4370</v>
       </c>
       <c r="E32" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="C33">
         <v>4370</v>
@@ -1423,15 +1419,15 @@
         <v>4370</v>
       </c>
       <c r="E33" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C34">
         <v>884</v>
@@ -1440,15 +1436,15 @@
         <v>884</v>
       </c>
       <c r="E34" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="C35">
         <v>785</v>
@@ -1457,15 +1453,15 @@
         <v>785</v>
       </c>
       <c r="E35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="C36">
         <v>4820</v>
@@ -1474,15 +1470,15 @@
         <v>4820</v>
       </c>
       <c r="E36" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="C37">
         <v>4766</v>
@@ -1491,15 +1487,15 @@
         <v>4766</v>
       </c>
       <c r="E37" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C38">
         <v>4074</v>
@@ -1508,15 +1504,15 @@
         <v>4074</v>
       </c>
       <c r="E38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>76</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>77</v>
       </c>
       <c r="C39">
         <v>4758</v>
@@ -1525,15 +1521,15 @@
         <v>4758</v>
       </c>
       <c r="E39" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="C40">
         <v>4439</v>
@@ -1542,15 +1538,15 @@
         <v>4439</v>
       </c>
       <c r="E40" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="C41">
         <v>4004</v>
@@ -1559,168 +1555,168 @@
         <v>4004</v>
       </c>
       <c r="E41" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42">
+        <v>1215</v>
+      </c>
+      <c r="D42">
+        <v>1215</v>
+      </c>
+      <c r="E42" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C42">
-        <v>1215</v>
-      </c>
-      <c r="D42">
-        <v>1215</v>
-      </c>
-      <c r="E42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43">
+        <v>1215</v>
+      </c>
+      <c r="D43">
+        <v>1215</v>
+      </c>
+      <c r="E43" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C43">
-        <v>1215</v>
-      </c>
-      <c r="D43">
-        <v>1215</v>
-      </c>
-      <c r="E43" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44">
+        <v>1215</v>
+      </c>
+      <c r="D44">
+        <v>1215</v>
+      </c>
+      <c r="E44" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C44">
-        <v>1215</v>
-      </c>
-      <c r="D44">
-        <v>1215</v>
-      </c>
-      <c r="E44" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45">
+        <v>1215</v>
+      </c>
+      <c r="D45">
+        <v>1215</v>
+      </c>
+      <c r="E45" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C45">
-        <v>1215</v>
-      </c>
-      <c r="D45">
-        <v>1215</v>
-      </c>
-      <c r="E45" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46">
+        <v>1215</v>
+      </c>
+      <c r="D46">
+        <v>1215</v>
+      </c>
+      <c r="E46" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C46">
-        <v>1215</v>
-      </c>
-      <c r="D46">
-        <v>1215</v>
-      </c>
-      <c r="E46" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47">
+        <v>1215</v>
+      </c>
+      <c r="D47">
+        <v>1215</v>
+      </c>
+      <c r="E47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C47">
-        <v>1215</v>
-      </c>
-      <c r="D47">
-        <v>1215</v>
-      </c>
-      <c r="E47" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="C48">
+        <v>5229</v>
+      </c>
+      <c r="D48">
+        <v>5229</v>
+      </c>
+      <c r="E48" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C48">
-        <v>5229</v>
-      </c>
-      <c r="D48">
-        <v>5229</v>
-      </c>
-      <c r="E48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="C49">
+        <v>5229</v>
+      </c>
+      <c r="D49">
+        <v>5229</v>
+      </c>
+      <c r="E49" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C49">
-        <v>5229</v>
-      </c>
-      <c r="D49">
-        <v>5229</v>
-      </c>
-      <c r="E49" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+      <c r="B50" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="C50">
+        <v>5229</v>
+      </c>
+      <c r="D50">
+        <v>5229</v>
+      </c>
+      <c r="E50" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C50">
-        <v>5229</v>
-      </c>
-      <c r="D50">
-        <v>5229</v>
-      </c>
-      <c r="E50" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="C51">
         <v>4393</v>
@@ -1729,15 +1725,15 @@
         <v>4393</v>
       </c>
       <c r="E51" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="C52">
         <v>4393</v>
@@ -1746,15 +1742,15 @@
         <v>4393</v>
       </c>
       <c r="E52" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="C53">
         <v>3903</v>
@@ -1763,15 +1759,15 @@
         <v>3903</v>
       </c>
       <c r="E53" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="C54">
         <v>3818</v>
@@ -1780,15 +1776,15 @@
         <v>3818</v>
       </c>
       <c r="E54" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="C55">
         <v>4680</v>
@@ -1797,15 +1793,15 @@
         <v>4680</v>
       </c>
       <c r="E55" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>111</v>
       </c>
       <c r="C56">
         <v>4679</v>
@@ -1814,15 +1810,15 @@
         <v>4679</v>
       </c>
       <c r="E56" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>113</v>
       </c>
       <c r="C57">
         <v>579</v>
@@ -1831,15 +1827,15 @@
         <v>579</v>
       </c>
       <c r="E57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="C58">
         <v>3174</v>
@@ -1848,15 +1844,15 @@
         <v>3174</v>
       </c>
       <c r="E58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="C59">
         <v>3205</v>
@@ -1865,15 +1861,15 @@
         <v>3205</v>
       </c>
       <c r="E59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="C60">
         <v>4965</v>
@@ -1882,15 +1878,15 @@
         <v>4965</v>
       </c>
       <c r="E60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="C61">
         <v>4956</v>
@@ -1899,15 +1895,15 @@
         <v>4956</v>
       </c>
       <c r="E61" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="C62">
         <v>3969</v>
@@ -1916,15 +1912,15 @@
         <v>3969</v>
       </c>
       <c r="E62" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>124</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>125</v>
       </c>
       <c r="C63">
         <v>3969</v>
@@ -1933,15 +1929,15 @@
         <v>3969</v>
       </c>
       <c r="E63" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="C64">
         <v>5497</v>
@@ -1950,15 +1946,15 @@
         <v>5497</v>
       </c>
       <c r="E64" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="C65">
         <v>5497</v>
@@ -1972,10 +1968,10 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="C66">
         <v>4416</v>
@@ -1984,15 +1980,15 @@
         <v>4416</v>
       </c>
       <c r="E66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>132</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>133</v>
       </c>
       <c r="C67">
         <v>4669</v>
@@ -2001,15 +1997,15 @@
         <v>4669</v>
       </c>
       <c r="E67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B68" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="B68" s="5" t="s">
-        <v>135</v>
       </c>
       <c r="C68">
         <v>4196</v>
@@ -2018,15 +2014,15 @@
         <v>4196</v>
       </c>
       <c r="E68" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="C69">
         <v>5090</v>
@@ -2035,17 +2031,11 @@
         <v>5090</v>
       </c>
       <c r="E69" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E69" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="S"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:E69" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>